<commit_message>
get lost two stations by adjust retrieve function
</commit_message>
<xml_diff>
--- a/data/am_tram17_name.xlsx
+++ b/data/am_tram17_name.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\UTNCE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3C65B7-CA3C-45B4-B4E0-5662F926090C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AE1CFE-6650-4A78-87C7-8D6ABCBBC3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40965" yWindow="2910" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Dijkgraafplein</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Witte de Withstraat</t>
   </si>
   <si>
-    <t>Nicolaas Beetsstraat</t>
-  </si>
-  <si>
     <t>Bilderdijkstraat</t>
   </si>
   <si>
@@ -88,18 +85,33 @@
   </si>
   <si>
     <t>Centraal Station_B</t>
+  </si>
+  <si>
+    <t>Jan Pieter Heijestraat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ten Katestraat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -127,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -405,120 +417,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>